<commit_message>
tabelas produtos e preços
</commit_message>
<xml_diff>
--- a/uteis/produtos_preco.xlsx
+++ b/uteis/produtos_preco.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego.rjoaquim\Desktop\app_tem_na_festa\uteis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AF2812-4531-49D9-A654-BF771EC44B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC7F267-490C-4899-AF87-26478FB01412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C085EA57-ED19-4FB0-87D0-2FDB0D578D0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C085EA57-ED19-4FB0-87D0-2FDB0D578D0C}"/>
   </bookViews>
   <sheets>
     <sheet name="CHURRASCO" sheetId="2" r:id="rId1"/>
+    <sheet name="FESTA" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="74">
   <si>
     <t>Tipo</t>
   </si>
@@ -44,12 +45,6 @@
     <t>Produto</t>
   </si>
   <si>
-    <t xml:space="preserve">Valor por grama </t>
-  </si>
-  <si>
-    <t>Valor quilograma / Litro</t>
-  </si>
-  <si>
     <t>Picanha</t>
   </si>
   <si>
@@ -258,6 +253,12 @@
   </si>
   <si>
     <t>Vinho</t>
+  </si>
+  <si>
+    <t>Valor por grama/ unidade</t>
+  </si>
+  <si>
+    <t>Valor quilograma / Litro / Garrafa/ Pacote/ Lata</t>
   </si>
 </sst>
 </file>
@@ -627,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC1559E-F7D9-4148-85E2-076A7498D389}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,8 +637,8 @@
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -645,585 +646,625 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC9FEC4-62A2-4C65-8887-16B72CEFC83C}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>